<commit_message>
Added validation / Used DTO's in controllers / increased the working speed of getLatestInfo()
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelFile.xlsx
+++ b/src/main/resources/ExcelFile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -32,28 +32,43 @@
     <t>City</t>
   </si>
   <si>
+    <t>few clouds</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:43:02.840109</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
     <t>clear sky</t>
   </si>
   <si>
-    <t>2025-07-18T15:50:54.472850</t>
+    <t>2025-07-18T22:43:02.971062</t>
   </si>
   <si>
     <t>Baku</t>
   </si>
   <si>
-    <t>broken clouds</t>
-  </si>
-  <si>
-    <t>2025-07-18T15:50:54.779901</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>2025-07-18T15:50:57.646235</t>
-  </si>
-  <si>
-    <t>2025-07-18T15:50:57.927312</t>
+    <t>2025-07-18T22:43:19.383522</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:43:19.492466</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:47:45.439110</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:47:45.581425</t>
+  </si>
+  <si>
+    <t>overcast clouds</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:47:45.691338</t>
+  </si>
+  <si>
+    <t>Moscow</t>
   </si>
 </sst>
 </file>
@@ -98,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -107,9 +122,9 @@
     <col min="1" max="1" width="2.640625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.46875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="8.26953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.23046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.36328125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="24.65234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.6171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.71484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -137,10 +152,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>31.4</v>
+        <v>23.09</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>44.0</v>
+        <v>71.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>6</v>
@@ -157,10 +172,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>22.9</v>
+        <v>24.03</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>66.0</v>
+        <v>73.0</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>9</v>
@@ -177,10 +192,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>31.4</v>
+        <v>23.09</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>44.0</v>
+        <v>71.0</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>6</v>
@@ -197,10 +212,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>22.9</v>
+        <v>24.03</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>66.0</v>
+        <v>73.0</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>9</v>
@@ -210,6 +225,66 @@
       </c>
       <c r="F5" t="s" s="0">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>22.95</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>71.0</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>24.03</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>73.0</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>19.24</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>58.0</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>